<commit_message>
controller and serviceImpl divide
</commit_message>
<xml_diff>
--- a/excelTest.xlsx
+++ b/excelTest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xehub\anyman\fileTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\anyman\excelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32106D-18C8-4034-B0F2-74546FDC5DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
-  <si>
-    <t>번호</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이름</t>
-  </si>
-  <si>
-    <t>이메일</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Fay</t>
   </si>
@@ -268,11 +257,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="000"/>
+    <numFmt numFmtId="176" formatCode="000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,12 +276,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <u/>
@@ -325,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -334,8 +317,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -650,562 +633,551 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.59765625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4" max="257" width="8.59765625" style="1"/>
-    <col min="258" max="259" width="8.3984375" style="1" customWidth="1"/>
-    <col min="260" max="513" width="8.59765625" style="1"/>
-    <col min="514" max="515" width="8.3984375" style="1" customWidth="1"/>
-    <col min="516" max="769" width="8.59765625" style="1"/>
-    <col min="770" max="771" width="8.3984375" style="1" customWidth="1"/>
-    <col min="772" max="1025" width="8.59765625" style="1"/>
-    <col min="1026" max="1027" width="8.3984375" style="1" customWidth="1"/>
-    <col min="1028" max="1281" width="8.59765625" style="1"/>
-    <col min="1282" max="1283" width="8.3984375" style="1" customWidth="1"/>
-    <col min="1284" max="1537" width="8.59765625" style="1"/>
-    <col min="1538" max="1539" width="8.3984375" style="1" customWidth="1"/>
-    <col min="1540" max="1793" width="8.59765625" style="1"/>
-    <col min="1794" max="1795" width="8.3984375" style="1" customWidth="1"/>
-    <col min="1796" max="2049" width="8.59765625" style="1"/>
-    <col min="2050" max="2051" width="8.3984375" style="1" customWidth="1"/>
-    <col min="2052" max="2305" width="8.59765625" style="1"/>
-    <col min="2306" max="2307" width="8.3984375" style="1" customWidth="1"/>
-    <col min="2308" max="2561" width="8.59765625" style="1"/>
-    <col min="2562" max="2563" width="8.3984375" style="1" customWidth="1"/>
-    <col min="2564" max="2817" width="8.59765625" style="1"/>
-    <col min="2818" max="2819" width="8.3984375" style="1" customWidth="1"/>
-    <col min="2820" max="3073" width="8.59765625" style="1"/>
-    <col min="3074" max="3075" width="8.3984375" style="1" customWidth="1"/>
-    <col min="3076" max="3329" width="8.59765625" style="1"/>
-    <col min="3330" max="3331" width="8.3984375" style="1" customWidth="1"/>
-    <col min="3332" max="3585" width="8.59765625" style="1"/>
-    <col min="3586" max="3587" width="8.3984375" style="1" customWidth="1"/>
-    <col min="3588" max="3841" width="8.59765625" style="1"/>
-    <col min="3842" max="3843" width="8.3984375" style="1" customWidth="1"/>
-    <col min="3844" max="4097" width="8.59765625" style="1"/>
-    <col min="4098" max="4099" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4100" max="4353" width="8.59765625" style="1"/>
-    <col min="4354" max="4355" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4356" max="4609" width="8.59765625" style="1"/>
-    <col min="4610" max="4611" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4612" max="4865" width="8.59765625" style="1"/>
-    <col min="4866" max="4867" width="8.3984375" style="1" customWidth="1"/>
-    <col min="4868" max="5121" width="8.59765625" style="1"/>
-    <col min="5122" max="5123" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5124" max="5377" width="8.59765625" style="1"/>
-    <col min="5378" max="5379" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5380" max="5633" width="8.59765625" style="1"/>
-    <col min="5634" max="5635" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5636" max="5889" width="8.59765625" style="1"/>
-    <col min="5890" max="5891" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5892" max="6145" width="8.59765625" style="1"/>
-    <col min="6146" max="6147" width="8.3984375" style="1" customWidth="1"/>
-    <col min="6148" max="6401" width="8.59765625" style="1"/>
-    <col min="6402" max="6403" width="8.3984375" style="1" customWidth="1"/>
-    <col min="6404" max="6657" width="8.59765625" style="1"/>
-    <col min="6658" max="6659" width="8.3984375" style="1" customWidth="1"/>
-    <col min="6660" max="6913" width="8.59765625" style="1"/>
-    <col min="6914" max="6915" width="8.3984375" style="1" customWidth="1"/>
-    <col min="6916" max="7169" width="8.59765625" style="1"/>
-    <col min="7170" max="7171" width="8.3984375" style="1" customWidth="1"/>
-    <col min="7172" max="7425" width="8.59765625" style="1"/>
-    <col min="7426" max="7427" width="8.3984375" style="1" customWidth="1"/>
-    <col min="7428" max="7681" width="8.59765625" style="1"/>
-    <col min="7682" max="7683" width="8.3984375" style="1" customWidth="1"/>
-    <col min="7684" max="7937" width="8.59765625" style="1"/>
-    <col min="7938" max="7939" width="8.3984375" style="1" customWidth="1"/>
-    <col min="7940" max="8193" width="8.59765625" style="1"/>
-    <col min="8194" max="8195" width="8.3984375" style="1" customWidth="1"/>
-    <col min="8196" max="8449" width="8.59765625" style="1"/>
-    <col min="8450" max="8451" width="8.3984375" style="1" customWidth="1"/>
-    <col min="8452" max="8705" width="8.59765625" style="1"/>
-    <col min="8706" max="8707" width="8.3984375" style="1" customWidth="1"/>
-    <col min="8708" max="8961" width="8.59765625" style="1"/>
-    <col min="8962" max="8963" width="8.3984375" style="1" customWidth="1"/>
-    <col min="8964" max="9217" width="8.59765625" style="1"/>
-    <col min="9218" max="9219" width="8.3984375" style="1" customWidth="1"/>
-    <col min="9220" max="9473" width="8.59765625" style="1"/>
-    <col min="9474" max="9475" width="8.3984375" style="1" customWidth="1"/>
-    <col min="9476" max="9729" width="8.59765625" style="1"/>
-    <col min="9730" max="9731" width="8.3984375" style="1" customWidth="1"/>
-    <col min="9732" max="9985" width="8.59765625" style="1"/>
-    <col min="9986" max="9987" width="8.3984375" style="1" customWidth="1"/>
-    <col min="9988" max="10241" width="8.59765625" style="1"/>
-    <col min="10242" max="10243" width="8.3984375" style="1" customWidth="1"/>
-    <col min="10244" max="10497" width="8.59765625" style="1"/>
-    <col min="10498" max="10499" width="8.3984375" style="1" customWidth="1"/>
-    <col min="10500" max="10753" width="8.59765625" style="1"/>
-    <col min="10754" max="10755" width="8.3984375" style="1" customWidth="1"/>
-    <col min="10756" max="11009" width="8.59765625" style="1"/>
-    <col min="11010" max="11011" width="8.3984375" style="1" customWidth="1"/>
-    <col min="11012" max="11265" width="8.59765625" style="1"/>
-    <col min="11266" max="11267" width="8.3984375" style="1" customWidth="1"/>
-    <col min="11268" max="11521" width="8.59765625" style="1"/>
-    <col min="11522" max="11523" width="8.3984375" style="1" customWidth="1"/>
-    <col min="11524" max="11777" width="8.59765625" style="1"/>
-    <col min="11778" max="11779" width="8.3984375" style="1" customWidth="1"/>
-    <col min="11780" max="12033" width="8.59765625" style="1"/>
-    <col min="12034" max="12035" width="8.3984375" style="1" customWidth="1"/>
-    <col min="12036" max="12289" width="8.59765625" style="1"/>
-    <col min="12290" max="12291" width="8.3984375" style="1" customWidth="1"/>
-    <col min="12292" max="12545" width="8.59765625" style="1"/>
-    <col min="12546" max="12547" width="8.3984375" style="1" customWidth="1"/>
-    <col min="12548" max="12801" width="8.59765625" style="1"/>
-    <col min="12802" max="12803" width="8.3984375" style="1" customWidth="1"/>
-    <col min="12804" max="13057" width="8.59765625" style="1"/>
-    <col min="13058" max="13059" width="8.3984375" style="1" customWidth="1"/>
-    <col min="13060" max="13313" width="8.59765625" style="1"/>
-    <col min="13314" max="13315" width="8.3984375" style="1" customWidth="1"/>
-    <col min="13316" max="13569" width="8.59765625" style="1"/>
-    <col min="13570" max="13571" width="8.3984375" style="1" customWidth="1"/>
-    <col min="13572" max="13825" width="8.59765625" style="1"/>
-    <col min="13826" max="13827" width="8.3984375" style="1" customWidth="1"/>
-    <col min="13828" max="14081" width="8.59765625" style="1"/>
-    <col min="14082" max="14083" width="8.3984375" style="1" customWidth="1"/>
-    <col min="14084" max="14337" width="8.59765625" style="1"/>
-    <col min="14338" max="14339" width="8.3984375" style="1" customWidth="1"/>
-    <col min="14340" max="14593" width="8.59765625" style="1"/>
-    <col min="14594" max="14595" width="8.3984375" style="1" customWidth="1"/>
-    <col min="14596" max="14849" width="8.59765625" style="1"/>
-    <col min="14850" max="14851" width="8.3984375" style="1" customWidth="1"/>
-    <col min="14852" max="15105" width="8.59765625" style="1"/>
-    <col min="15106" max="15107" width="8.3984375" style="1" customWidth="1"/>
-    <col min="15108" max="15361" width="8.59765625" style="1"/>
-    <col min="15362" max="15363" width="8.3984375" style="1" customWidth="1"/>
-    <col min="15364" max="15617" width="8.59765625" style="1"/>
-    <col min="15618" max="15619" width="8.3984375" style="1" customWidth="1"/>
-    <col min="15620" max="15873" width="8.59765625" style="1"/>
-    <col min="15874" max="15875" width="8.3984375" style="1" customWidth="1"/>
-    <col min="15876" max="16129" width="8.59765625" style="1"/>
-    <col min="16130" max="16131" width="8.3984375" style="1" customWidth="1"/>
-    <col min="16132" max="16384" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="30.625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="8.375" style="1" customWidth="1"/>
+    <col min="4" max="257" width="8.625" style="1"/>
+    <col min="258" max="259" width="8.375" style="1" customWidth="1"/>
+    <col min="260" max="513" width="8.625" style="1"/>
+    <col min="514" max="515" width="8.375" style="1" customWidth="1"/>
+    <col min="516" max="769" width="8.625" style="1"/>
+    <col min="770" max="771" width="8.375" style="1" customWidth="1"/>
+    <col min="772" max="1025" width="8.625" style="1"/>
+    <col min="1026" max="1027" width="8.375" style="1" customWidth="1"/>
+    <col min="1028" max="1281" width="8.625" style="1"/>
+    <col min="1282" max="1283" width="8.375" style="1" customWidth="1"/>
+    <col min="1284" max="1537" width="8.625" style="1"/>
+    <col min="1538" max="1539" width="8.375" style="1" customWidth="1"/>
+    <col min="1540" max="1793" width="8.625" style="1"/>
+    <col min="1794" max="1795" width="8.375" style="1" customWidth="1"/>
+    <col min="1796" max="2049" width="8.625" style="1"/>
+    <col min="2050" max="2051" width="8.375" style="1" customWidth="1"/>
+    <col min="2052" max="2305" width="8.625" style="1"/>
+    <col min="2306" max="2307" width="8.375" style="1" customWidth="1"/>
+    <col min="2308" max="2561" width="8.625" style="1"/>
+    <col min="2562" max="2563" width="8.375" style="1" customWidth="1"/>
+    <col min="2564" max="2817" width="8.625" style="1"/>
+    <col min="2818" max="2819" width="8.375" style="1" customWidth="1"/>
+    <col min="2820" max="3073" width="8.625" style="1"/>
+    <col min="3074" max="3075" width="8.375" style="1" customWidth="1"/>
+    <col min="3076" max="3329" width="8.625" style="1"/>
+    <col min="3330" max="3331" width="8.375" style="1" customWidth="1"/>
+    <col min="3332" max="3585" width="8.625" style="1"/>
+    <col min="3586" max="3587" width="8.375" style="1" customWidth="1"/>
+    <col min="3588" max="3841" width="8.625" style="1"/>
+    <col min="3842" max="3843" width="8.375" style="1" customWidth="1"/>
+    <col min="3844" max="4097" width="8.625" style="1"/>
+    <col min="4098" max="4099" width="8.375" style="1" customWidth="1"/>
+    <col min="4100" max="4353" width="8.625" style="1"/>
+    <col min="4354" max="4355" width="8.375" style="1" customWidth="1"/>
+    <col min="4356" max="4609" width="8.625" style="1"/>
+    <col min="4610" max="4611" width="8.375" style="1" customWidth="1"/>
+    <col min="4612" max="4865" width="8.625" style="1"/>
+    <col min="4866" max="4867" width="8.375" style="1" customWidth="1"/>
+    <col min="4868" max="5121" width="8.625" style="1"/>
+    <col min="5122" max="5123" width="8.375" style="1" customWidth="1"/>
+    <col min="5124" max="5377" width="8.625" style="1"/>
+    <col min="5378" max="5379" width="8.375" style="1" customWidth="1"/>
+    <col min="5380" max="5633" width="8.625" style="1"/>
+    <col min="5634" max="5635" width="8.375" style="1" customWidth="1"/>
+    <col min="5636" max="5889" width="8.625" style="1"/>
+    <col min="5890" max="5891" width="8.375" style="1" customWidth="1"/>
+    <col min="5892" max="6145" width="8.625" style="1"/>
+    <col min="6146" max="6147" width="8.375" style="1" customWidth="1"/>
+    <col min="6148" max="6401" width="8.625" style="1"/>
+    <col min="6402" max="6403" width="8.375" style="1" customWidth="1"/>
+    <col min="6404" max="6657" width="8.625" style="1"/>
+    <col min="6658" max="6659" width="8.375" style="1" customWidth="1"/>
+    <col min="6660" max="6913" width="8.625" style="1"/>
+    <col min="6914" max="6915" width="8.375" style="1" customWidth="1"/>
+    <col min="6916" max="7169" width="8.625" style="1"/>
+    <col min="7170" max="7171" width="8.375" style="1" customWidth="1"/>
+    <col min="7172" max="7425" width="8.625" style="1"/>
+    <col min="7426" max="7427" width="8.375" style="1" customWidth="1"/>
+    <col min="7428" max="7681" width="8.625" style="1"/>
+    <col min="7682" max="7683" width="8.375" style="1" customWidth="1"/>
+    <col min="7684" max="7937" width="8.625" style="1"/>
+    <col min="7938" max="7939" width="8.375" style="1" customWidth="1"/>
+    <col min="7940" max="8193" width="8.625" style="1"/>
+    <col min="8194" max="8195" width="8.375" style="1" customWidth="1"/>
+    <col min="8196" max="8449" width="8.625" style="1"/>
+    <col min="8450" max="8451" width="8.375" style="1" customWidth="1"/>
+    <col min="8452" max="8705" width="8.625" style="1"/>
+    <col min="8706" max="8707" width="8.375" style="1" customWidth="1"/>
+    <col min="8708" max="8961" width="8.625" style="1"/>
+    <col min="8962" max="8963" width="8.375" style="1" customWidth="1"/>
+    <col min="8964" max="9217" width="8.625" style="1"/>
+    <col min="9218" max="9219" width="8.375" style="1" customWidth="1"/>
+    <col min="9220" max="9473" width="8.625" style="1"/>
+    <col min="9474" max="9475" width="8.375" style="1" customWidth="1"/>
+    <col min="9476" max="9729" width="8.625" style="1"/>
+    <col min="9730" max="9731" width="8.375" style="1" customWidth="1"/>
+    <col min="9732" max="9985" width="8.625" style="1"/>
+    <col min="9986" max="9987" width="8.375" style="1" customWidth="1"/>
+    <col min="9988" max="10241" width="8.625" style="1"/>
+    <col min="10242" max="10243" width="8.375" style="1" customWidth="1"/>
+    <col min="10244" max="10497" width="8.625" style="1"/>
+    <col min="10498" max="10499" width="8.375" style="1" customWidth="1"/>
+    <col min="10500" max="10753" width="8.625" style="1"/>
+    <col min="10754" max="10755" width="8.375" style="1" customWidth="1"/>
+    <col min="10756" max="11009" width="8.625" style="1"/>
+    <col min="11010" max="11011" width="8.375" style="1" customWidth="1"/>
+    <col min="11012" max="11265" width="8.625" style="1"/>
+    <col min="11266" max="11267" width="8.375" style="1" customWidth="1"/>
+    <col min="11268" max="11521" width="8.625" style="1"/>
+    <col min="11522" max="11523" width="8.375" style="1" customWidth="1"/>
+    <col min="11524" max="11777" width="8.625" style="1"/>
+    <col min="11778" max="11779" width="8.375" style="1" customWidth="1"/>
+    <col min="11780" max="12033" width="8.625" style="1"/>
+    <col min="12034" max="12035" width="8.375" style="1" customWidth="1"/>
+    <col min="12036" max="12289" width="8.625" style="1"/>
+    <col min="12290" max="12291" width="8.375" style="1" customWidth="1"/>
+    <col min="12292" max="12545" width="8.625" style="1"/>
+    <col min="12546" max="12547" width="8.375" style="1" customWidth="1"/>
+    <col min="12548" max="12801" width="8.625" style="1"/>
+    <col min="12802" max="12803" width="8.375" style="1" customWidth="1"/>
+    <col min="12804" max="13057" width="8.625" style="1"/>
+    <col min="13058" max="13059" width="8.375" style="1" customWidth="1"/>
+    <col min="13060" max="13313" width="8.625" style="1"/>
+    <col min="13314" max="13315" width="8.375" style="1" customWidth="1"/>
+    <col min="13316" max="13569" width="8.625" style="1"/>
+    <col min="13570" max="13571" width="8.375" style="1" customWidth="1"/>
+    <col min="13572" max="13825" width="8.625" style="1"/>
+    <col min="13826" max="13827" width="8.375" style="1" customWidth="1"/>
+    <col min="13828" max="14081" width="8.625" style="1"/>
+    <col min="14082" max="14083" width="8.375" style="1" customWidth="1"/>
+    <col min="14084" max="14337" width="8.625" style="1"/>
+    <col min="14338" max="14339" width="8.375" style="1" customWidth="1"/>
+    <col min="14340" max="14593" width="8.625" style="1"/>
+    <col min="14594" max="14595" width="8.375" style="1" customWidth="1"/>
+    <col min="14596" max="14849" width="8.625" style="1"/>
+    <col min="14850" max="14851" width="8.375" style="1" customWidth="1"/>
+    <col min="14852" max="15105" width="8.625" style="1"/>
+    <col min="15106" max="15107" width="8.375" style="1" customWidth="1"/>
+    <col min="15108" max="15361" width="8.625" style="1"/>
+    <col min="15362" max="15363" width="8.375" style="1" customWidth="1"/>
+    <col min="15364" max="15617" width="8.625" style="1"/>
+    <col min="15618" max="15619" width="8.375" style="1" customWidth="1"/>
+    <col min="15620" max="15873" width="8.625" style="1"/>
+    <col min="15874" max="15875" width="8.375" style="1" customWidth="1"/>
+    <col min="15876" max="16129" width="8.625" style="1"/>
+    <col min="16130" max="16131" width="8.375" style="1" customWidth="1"/>
+    <col min="16132" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" s="3">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" s="3">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" s="3">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" s="3">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C33" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C35" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C36" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C31" r:id="rId1"/>
+    <hyperlink ref="C32" r:id="rId2"/>
+    <hyperlink ref="C33" r:id="rId3"/>
+    <hyperlink ref="C34" r:id="rId4"/>
+    <hyperlink ref="C35" r:id="rId5"/>
+    <hyperlink ref="C36" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>

</xml_diff>